<commit_message>
Deploying to gh-pages from @ tech-acs/crvsreportpackage@38449519750198f939ebd797c0ef0be1530eebbc 🚀
</commit_message>
<xml_diff>
--- a/reference/output.xlsx
+++ b/reference/output.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A74"/>
+  <dimension ref="A1:A75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -479,397 +479,404 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/styling_tables.html"&gt;Creating publication-ready tables&lt;/a&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
+          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>&lt;li class="nav-item dropdown"&gt;</t>
+          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
+          <t>&lt;li class="nav-item dropdown"&gt;</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/div&gt;</t>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;/ul&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>&lt;div class="row"&gt;</t>
+          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
+          <t>&lt;div class="row"&gt;</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
+          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
+          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>&lt;div class="ref-description section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
+          <t>&lt;div class="ref-description section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
+          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
+          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>&lt;/dl&gt;&lt;/div&gt;</t>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/dl&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
+          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
+          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
+          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
+          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
+          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
+          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>&lt;/footer&gt;&lt;/div&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
+        <is>
+          <t>&lt;/footer&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
         <is>
           <t>&lt;/body&gt;&lt;/html&gt;</t>
         </is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ tech-acs/crvsreportpackage@87b8366f4597f952e33b430ab7b8515cb724e2e9 🚀
</commit_message>
<xml_diff>
--- a/reference/output.xlsx
+++ b/reference/output.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A75"/>
+  <dimension ref="A1:A76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,397 +486,404 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/choropleth_maps.html"&gt;Creating choropleth maps&lt;/a&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
+          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>&lt;li class="nav-item dropdown"&gt;</t>
+          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
+          <t>&lt;li class="nav-item dropdown"&gt;</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/div&gt;</t>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;/ul&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>&lt;div class="row"&gt;</t>
+          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
+          <t>&lt;div class="row"&gt;</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
+          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
+          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>&lt;div class="ref-description section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
+          <t>&lt;div class="ref-description section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
+          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
+          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>&lt;/dl&gt;&lt;/div&gt;</t>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/dl&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
+          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
+          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
+          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
+          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
+          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
+          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>&lt;/footer&gt;&lt;/div&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
+        <is>
+          <t>&lt;/footer&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
         <is>
           <t>&lt;/body&gt;&lt;/html&gt;</t>
         </is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ tech-acs/crvsreportpackage@e7cec764e0ca357b23fd7361d6eb288613775833 🚀
</commit_message>
<xml_diff>
--- a/reference/output.xlsx
+++ b/reference/output.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A76"/>
+  <dimension ref="A1:A73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,7 +395,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>&lt;small class="nav-text text-muted me-auto" data-bs-toggle="tooltip" data-bs-placement="bottom" title=""&gt;0.2.3&lt;/small&gt;</t>
+          <t>&lt;small class="nav-text text-muted me-auto" data-bs-toggle="tooltip" data-bs-placement="bottom" title=""&gt;0.2.4&lt;/small&gt;</t>
         </is>
       </c>
     </row>
@@ -458,147 +458,147 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>&lt;ul class="dropdown-menu" aria-labelledby="dropdown-articles"&gt;&lt;li&gt;&lt;a class="dropdown-item" href="../articles/data_cleaning.html"&gt;Data cleaning&lt;/a&gt;&lt;/li&gt;</t>
+          <t>&lt;ul class="dropdown-menu" aria-labelledby="dropdown-articles"&gt;&lt;li&gt;&lt;a class="dropdown-item" href="../articles/data_mapping.html"&gt;Mapping variables to outputs&lt;/a&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/data_mapping.html"&gt;Mapping variables to outputs&lt;/a&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/table_templates.html"&gt;CRVS tables&lt;/a&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/table_templates.html"&gt;CRVS tables&lt;/a&gt;&lt;/li&gt;</t>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/styling_tables.html"&gt;Creating publication-ready tables&lt;/a&gt;&lt;/li&gt;</t>
+          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/choropleth_maps.html"&gt;Creating choropleth maps&lt;/a&gt;&lt;/li&gt;</t>
+          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+          <t>&lt;li class="nav-item dropdown"&gt;</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
+          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
+          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>&lt;li class="nav-item dropdown"&gt;</t>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;/ul&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/div&gt;</t>
+          <t>&lt;div class="row"&gt;</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
+          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>&lt;div class="row"&gt;</t>
+          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
+          <t>&lt;div class="ref-description section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
+          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -612,238 +612,238 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>&lt;div class="ref-description section level2"&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
+          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
+          <t>&lt;/dl&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
+          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>&lt;/dl&gt;&lt;/div&gt;</t>
+          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
+          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
+          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
+          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
+          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
+          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -857,33 +857,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
+          <t>&lt;/footer&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>&lt;/div&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>&lt;/footer&gt;&lt;/div&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
         <is>
           <t>&lt;/body&gt;&lt;/html&gt;</t>
         </is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ tech-acs/crvsreportpackage@4b01c63c4e0e69800ec24fb1cfea889709017625 🚀
</commit_message>
<xml_diff>
--- a/reference/output.xlsx
+++ b/reference/output.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A73"/>
+  <dimension ref="A1:A74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -458,411 +458,418 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>&lt;ul class="dropdown-menu" aria-labelledby="dropdown-articles"&gt;&lt;li&gt;&lt;a class="dropdown-item" href="../articles/data_mapping.html"&gt;Mapping variables to outputs&lt;/a&gt;&lt;/li&gt;</t>
+          <t>&lt;ul class="dropdown-menu" aria-labelledby="dropdown-articles"&gt;&lt;li&gt;&lt;a class="dropdown-item" href="../articles/developer_manual.html"&gt;Developer Manual&lt;/a&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/table_templates.html"&gt;CRVS tables&lt;/a&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/data_mapping.html"&gt;Mapping variables to outputs&lt;/a&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/table_templates.html"&gt;CRVS tables&lt;/a&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
+          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>&lt;li class="nav-item dropdown"&gt;</t>
+          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
+          <t>&lt;li class="nav-item dropdown"&gt;</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>&lt;/ul&gt;&lt;/div&gt;</t>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;/ul&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>&lt;div class="row"&gt;</t>
+          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
+          <t>&lt;div class="row"&gt;</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
+          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
+          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>&lt;div class="ref-description section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
+          <t>&lt;div class="ref-description section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
+          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
+          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>&lt;/dl&gt;&lt;/div&gt;</t>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/dl&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
+          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>&lt;div class="section level2"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+          <t>&lt;div class="section level2"&gt;</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
+          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
+          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
+          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
+          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
+          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>&lt;/div&gt;</t>
+          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>&lt;/footer&gt;&lt;/div&gt;</t>
+          <t>&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
+        <is>
+          <t>&lt;/footer&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
         <is>
           <t>&lt;/body&gt;&lt;/html&gt;</t>
         </is>

</xml_diff>